<commit_message>
Update Backlog (new sheet added for tp2)
</commit_message>
<xml_diff>
--- a/Backlog/Backlog.xlsx
+++ b/Backlog/Backlog.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Williams\OneDrive\Bureau\Cours Ing3\Architecure distribuee\tp-paas-portique\Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1A9332-33A4-47C2-BCA4-103D3AB23150}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A3D80F8-F623-4406-AC3C-EC7DAA44D33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
+    <sheet name="Product Backlog TP1" sheetId="1" r:id="rId1"/>
+    <sheet name="TP2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="157">
   <si>
     <t>Titre</t>
   </si>
@@ -426,6 +427,87 @@
   </si>
   <si>
     <t>Clément</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watchdog </t>
+  </si>
+  <si>
+    <t>Implémentation du watchdog pour les 2 services core-backend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud SQL </t>
+  </si>
+  <si>
+    <t>Membre</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo associée au badge </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Replication Core-one/Core-Two </t>
+  </si>
+  <si>
+    <t>Séparation Back-one</t>
+  </si>
+  <si>
+    <t>Réplication des services Core</t>
+  </si>
+  <si>
+    <t>Création d'un backend qui permet d'appeler Core-one/Core-two selon la disponibilité</t>
+  </si>
+  <si>
+    <t>Docker Swarm</t>
+  </si>
+  <si>
+    <t>Implémentation d'un système de CI/CD et de gestion des fichiers de config via Docker Swarm</t>
+  </si>
+  <si>
+    <t>Clusterisation Redis</t>
+  </si>
+  <si>
+    <t>Création d'un cluster Redis avec un Master et un Slave qui synchronisent les données</t>
+  </si>
+  <si>
+    <t>Utilisation d'une base PostgreSQL directement depuis le cloud (GCP)</t>
+  </si>
+  <si>
+    <t>Création d'un service qui stocke les images et les met à disposition via une API (Request GET)</t>
+  </si>
+  <si>
+    <t>Récupération des Images</t>
+  </si>
+  <si>
+    <t>Appel à l'API du service qui stocke les images et affichage sur le Front</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Composant </t>
+  </si>
+  <si>
+    <t>Watchdog</t>
+  </si>
+  <si>
+    <t>Base de données</t>
+  </si>
+  <si>
+    <t>Photo Storage Service</t>
+  </si>
+  <si>
+    <t>Core-one/Core-two</t>
+  </si>
+  <si>
+    <t>Back-one</t>
+  </si>
+  <si>
+    <t>Redis</t>
+  </si>
+  <si>
+    <t>CI/CD</t>
+  </si>
+  <si>
+    <t>Static-Server-Backend</t>
   </si>
 </sst>
 </file>
@@ -607,7 +689,63 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="25">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF008000"/>
+          <bgColor rgb="FF008000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF32CD32"/>
+          <bgColor rgb="FF32CD32"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF87CEEB"/>
+          <bgColor rgb="FF87CEEB"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4A460"/>
+          <bgColor rgb="FFF4A460"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFD700"/>
+          <bgColor rgb="FFFFD700"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -778,16 +916,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D643792-BA16-4AF4-A20C-C9DB4EE7EB3E}" name="Tableau1" displayName="Tableau1" ref="A1:G35" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2D643792-BA16-4AF4-A20C-C9DB4EE7EB3E}" name="Tableau1" displayName="Tableau1" ref="A1:G35" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21">
   <autoFilter ref="A1:G35" xr:uid="{2D643792-BA16-4AF4-A20C-C9DB4EE7EB3E}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{930B0FC4-07FF-4BEE-B107-1988AB2AED2D}" name="Titre" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{B4FAA37D-B1CD-4E55-805A-4E360AEE36D8}" name="Composant" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{45B2F884-034A-46FC-84A0-EAA5D9E8A3C4}" name="Description" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{67DBA196-99B9-49B0-8D8F-A9E33B07B73A}" name="Priorité" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{ADA11A62-F794-4FD6-9942-8B150C1916B5}" name="Charge" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{952E9D4E-95FB-4079-8817-A3FC45FD189A}" name="Developpé par" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{58DE0A7F-371B-4DB8-9E8E-F135523EBA7D}" name="Statut" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{930B0FC4-07FF-4BEE-B107-1988AB2AED2D}" name="Titre" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{B4FAA37D-B1CD-4E55-805A-4E360AEE36D8}" name="Composant" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{45B2F884-034A-46FC-84A0-EAA5D9E8A3C4}" name="Description" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{67DBA196-99B9-49B0-8D8F-A9E33B07B73A}" name="Priorité" dataDxfId="17"/>
+    <tableColumn id="5" xr3:uid="{ADA11A62-F794-4FD6-9942-8B150C1916B5}" name="Charge" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{952E9D4E-95FB-4079-8817-A3FC45FD189A}" name="Developpé par" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{58DE0A7F-371B-4DB8-9E8E-F135523EBA7D}" name="Statut" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1080,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1"/>
@@ -1906,38 +2044,38 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G112">
-    <cfRule type="expression" dxfId="6" priority="1">
+  <conditionalFormatting sqref="G41:G112 G2:G38">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>$G2="À faire"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>$G2="En cours"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="11" priority="3">
       <formula>$G2="En revue"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>$G2="En test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>$G2="Bloqué"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>$G2="Fait"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="7">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>$G2="Déployé"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F28" xr:uid="{EF99E562-5672-4513-85FC-BDEFB56AB771}">
-      <formula1>$M$5:$M$9</formula1>
-    </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2:G33" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"À faire,En cours,En revue,En test,Bloqué,Fait"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2:G33" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"À faire,En cours,En revue,En test,Bloqué,Fait,Déployé"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F28" xr:uid="{EF99E562-5672-4513-85FC-BDEFB56AB771}">
+      <formula1>$M$5:$M$9</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1947,7 +2085,218 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C39403-DB42-4296-85D1-8948BBD6901D}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="28.21875" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="77.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" customHeight="1">
+      <c r="A3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" customHeight="1">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>135</v>
+      </c>
+      <c r="B5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" t="s">
+        <v>154</v>
+      </c>
+      <c r="C9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B10" t="s">
+        <v>156</v>
+      </c>
+      <c r="C10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E3:E10">
+    <cfRule type="expression" dxfId="6" priority="15">
+      <formula>$E3="À faire"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="16">
+      <formula>$E3="En cours"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="17">
+      <formula>$E3="En revue"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="18">
+      <formula>$E3="En test"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="19">
+      <formula>$E3="Bloqué"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="20">
+      <formula>$E3="Fait"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="21">
+      <formula>$E3="Déployé"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D7060A2D58E54441AB4F87107E68FC2B" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8049f48f8bc13cb6ae80ac851ae97c91">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c3aedc28-128d-481c-b801-24d0b8bf0390" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d88346d1a9845869c53c9eee838b7150" ns2:_="">
     <xsd:import namespace="c3aedc28-128d-481c-b801-24d0b8bf0390"/>
@@ -2117,22 +2466,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{267433CF-B0BD-450F-BE35-AB892440A25E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{472F63C7-E95F-4904-A5A3-6AE8CC4358D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6681C706-DD0F-4D94-8DB9-C740D502D661}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2148,21 +2499,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{472F63C7-E95F-4904-A5A3-6AE8CC4358D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{267433CF-B0BD-450F-BE35-AB892440A25E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>